<commit_message>
redesign of avionics bay nearly done, parachute detainment designed as well
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\BadIdeaRocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156D21D8-ED70-4FB3-9125-14473351473D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917B3E7E-D0B6-486A-B11D-58361F79CBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>TASK</t>
   </si>
@@ -94,13 +94,31 @@
   </si>
   <si>
     <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Planning on printing new fin guide soon</t>
+  </si>
+  <si>
+    <t>Printing new motor mount screwhole guide OCT 17</t>
+  </si>
+  <si>
+    <t>Issue was due to motor mount screwholes interfering with coupler pegs. This has been fixed and current coupler design is acceptable.</t>
+  </si>
+  <si>
+    <t>Everything should fit, need to double check once I get components. Also unsure if I can stack MOSFET boards but that's the plan rn. INCLUDE SERVO (forgot)</t>
+  </si>
+  <si>
+    <t>All the way back here since I'm waiting on components from China</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +147,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +177,11 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -162,23 +192,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -461,7 +495,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,15 +520,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="7">
         <v>44851</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -521,6 +555,9 @@
       <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -533,20 +570,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>44856</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>44860</v>
@@ -554,21 +594,27 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7">
         <v>44860</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3">
         <v>44860</v>
@@ -576,13 +622,14 @@
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3">
-        <v>44860</v>
+        <v>44865</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
@@ -590,7 +637,7 @@
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>44865</v>
@@ -601,7 +648,7 @@
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3">
         <v>44865</v>
@@ -612,7 +659,7 @@
     </row>
     <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>44865</v>
@@ -623,10 +670,10 @@
     </row>
     <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3">
-        <v>44865</v>
+        <v>44870</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
@@ -634,10 +681,10 @@
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3">
-        <v>44867</v>
+        <v>44870</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
@@ -645,29 +692,32 @@
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3">
-        <v>44870</v>
+        <v>44871</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
-        <v>44870</v>
+        <v>44877</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D18">
-    <sortCondition ref="B1:B18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
+    <sortCondition ref="B1:B17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TODO: finish blast shield and potentially flip servo mount
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\BadIdeaRocket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\OneDrive - University of Ottawa\Documents\BadIdeaRocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917B3E7E-D0B6-486A-B11D-58361F79CBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332E4620-79CE-4641-B9D6-B2A8EDE0C9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>TASK</t>
   </si>
@@ -108,10 +108,16 @@
     <t>Issue was due to motor mount screwholes interfering with coupler pegs. This has been fixed and current coupler design is acceptable.</t>
   </si>
   <si>
-    <t>Everything should fit, need to double check once I get components. Also unsure if I can stack MOSFET boards but that's the plan rn. INCLUDE SERVO (forgot)</t>
-  </si>
-  <si>
     <t>All the way back here since I'm waiting on components from China</t>
+  </si>
+  <si>
+    <t>Everything should fit, need to double check once I get components. Accidentally modeled servo retention on wrong side of tube I think, gotta flip it</t>
+  </si>
+  <si>
+    <t>Blast shield redesigned to two piece unit with wire passthrough. Need to CAD screwholes and then should be good to install</t>
+  </si>
+  <si>
+    <t>Prototype designed and retaining servo integrated in avionics bay. Testing tbd</t>
   </si>
 </sst>
 </file>
@@ -494,19 +500,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="183.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.69140625" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="183.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -520,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -531,7 +537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -556,21 +562,24 @@
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>44856</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -584,7 +593,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -598,7 +607,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -612,7 +621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -624,18 +633,21 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>44865</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -646,7 +658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -657,7 +669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -668,7 +680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -679,7 +691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -690,7 +702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -701,10 +713,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>